<commit_message>
IIS URL Rewriter hinzugefügt
Installationsvoraussetzung für IIS URL Rewriter Modul hinzugefügt
</commit_message>
<xml_diff>
--- a/Exchange Server 2019 Setup.xlsx
+++ b/Exchange Server 2019 Setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\SetupExchangeServer2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18305F9F-DA2F-4511-A035-B30B8EBDF6BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD1C037-5979-4979-ADCB-4AF3707AFAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="142">
   <si>
     <t>Plattform</t>
   </si>
@@ -732,9 +732,6 @@
     <t>Installation von Exchange Server 2019</t>
   </si>
   <si>
-    <t>Setup.exe /Mode:Install /Roles:Mailbox /IAcceptExchangeServerLicenseTerms</t>
-  </si>
-  <si>
     <t>4.2</t>
   </si>
   <si>
@@ -808,9 +805,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
   <si>
     <t>https://go.granikos.eu/2NfPkvR</t>
@@ -829,12 +823,6 @@
     <t>1.11</t>
   </si>
   <si>
-    <t>Konfiguration der DSN Einträge in der internen und externen DNS-Zone, z.B.
-autodiscover.varunagroup.de -&gt; A Record
-mail.varunagoup.de -&gt; A Record
-download.varunagroup.de -&gt; CNAME auf mail.varunagroup.de</t>
-  </si>
-  <si>
     <t>Kommandos</t>
   </si>
   <si>
@@ -851,13 +839,32 @@
   </si>
   <si>
     <t>https://msrc.microsoft.com/update-guide/vulnerability/CVE-2021-1730</t>
+  </si>
+  <si>
+    <t>Konfiguration der DNS Einträge in der internen und externen DNS-Zone, z.B.
+autodiscover.varunagroup.de -&gt; A Record
+mail.varunagoup.de -&gt; A Record
+download.varunagroup.de -&gt; CNAME auf mail.varunagroup.de</t>
+  </si>
+  <si>
+    <t>Download IIS URL Rewriter-Modul</t>
+  </si>
+  <si>
+    <t>https://www.iis.net/downloads/microsoft/url-rewrite#additionalDownloads</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>Setup.exe /Mode:Install /Roles:Mailbox /IAcceptExchangeServerLicenseTerms_DiagnosticDataON
+Setup.exe /Mode:Install /Roles:Mailbox /IAcceptExchangeServerLicenseTerms_DiagnosticDataOFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,6 +970,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1034,7 +1048,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
@@ -1105,6 +1119,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40 % - Akzent4" xfId="3" builtinId="43"/>
@@ -1134,13 +1153,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1495,26 +1514,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B25"/>
+  <dimension ref="A2:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="29"/>
     </row>
-    <row r="3" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -1522,16 +1541,16 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="29"/>
     </row>
-    <row r="6" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1539,24 +1558,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="23">
-        <v>43952</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>3</v>
       </c>
@@ -1564,17 +1583,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="str">
         <f>Lookup!A3</f>
         <v>Nicht begonnen</v>
       </c>
       <c r="B14" s="25">
         <f>COUNTIF('Installation Exchange 2019'!D:D,Lookup!A3)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="str">
         <f>Lookup!A4</f>
         <v>In Ausführung</v>
@@ -1584,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="str">
         <f>Lookup!A5</f>
         <v>Abgeschlossen</v>
@@ -1594,12 +1613,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" t="s">
-        <v>129</v>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="32">
+        <v>44486</v>
       </c>
     </row>
   </sheetData>
@@ -1615,24 +1642,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CACAE57-EC22-477C-B012-303C9CEF819F}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView topLeftCell="E37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="13" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.453125" customWidth="1"/>
-    <col min="7" max="7" width="102.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.42578125" customWidth="1"/>
+    <col min="7" max="7" width="102.140625" customWidth="1"/>
     <col min="8" max="8" width="102" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1652,13 +1679,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5">
@@ -1673,12 +1700,12 @@
       <c r="H2" s="4"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="9" t="str">
-        <f t="shared" ref="B3:B13" si="0">ExchangeTeam</f>
+        <f t="shared" ref="B3:B14" si="0">ExchangeTeam</f>
         <v>John Doe</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1688,19 +1715,19 @@
         <v>8</v>
       </c>
       <c r="E3" s="11">
-        <f t="shared" ref="E3:E13" si="1">StartDate</f>
-        <v>43952</v>
+        <f t="shared" ref="E3:E14" si="1">StartDate</f>
+        <v>44531</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
@@ -1716,15 +1743,15 @@
       </c>
       <c r="E4" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="13"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -1740,7 +1767,7 @@
       </c>
       <c r="E5" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>41</v>
@@ -1751,7 +1778,7 @@
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
@@ -1767,7 +1794,7 @@
       </c>
       <c r="E6" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>43</v>
@@ -1778,7 +1805,7 @@
       </c>
       <c r="L6" s="14"/>
     </row>
-    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -1794,7 +1821,7 @@
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>45</v>
@@ -1805,7 +1832,7 @@
       </c>
       <c r="L7" s="14"/>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
@@ -1821,7 +1848,7 @@
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>48</v>
@@ -1832,7 +1859,7 @@
       </c>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
@@ -1848,18 +1875,18 @@
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="16" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
@@ -1875,18 +1902,18 @@
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="16" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -1902,14 +1929,18 @@
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="H11" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -1918,21 +1949,21 @@
         <v>John Doe</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>134</v>
+        <v>44531</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
@@ -1941,85 +1972,82 @@
         <v>John Doe</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="1:12" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>John Doe</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="1"/>
+        <v>44531</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="4" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="9" t="str">
-        <f t="shared" ref="B15:B27" si="2">ExchangeTeam</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f t="shared" ref="B16:B28" si="2">ExchangeTeam</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="11">
-        <f t="shared" ref="E15:E27" si="3">StartDate</f>
-        <v>43952</v>
-      </c>
-      <c r="F15" s="18" t="s">
+      <c r="D16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" ref="E16:E28" si="3">StartDate</f>
+        <v>44531</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>John Doe</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="11">
-        <f t="shared" si="3"/>
-        <v>43952</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="G16" s="13"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="1:8" s="12" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>29</v>
       </c>
@@ -2028,24 +2056,24 @@
         <v>John Doe</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>29</v>
       </c>
@@ -2054,22 +2082,24 @@
         <v>John Doe</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -2078,22 +2108,22 @@
         <v>John Doe</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>29</v>
       </c>
@@ -2102,24 +2132,22 @@
         <v>John Doe</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G20" s="17"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -2128,22 +2156,24 @@
         <v>John Doe</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="H21" s="16"/>
     </row>
-    <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
@@ -2152,22 +2182,22 @@
         <v>John Doe</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -2176,24 +2206,22 @@
         <v>John Doe</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G23" s="17"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>29</v>
       </c>
@@ -2202,22 +2230,24 @@
         <v>John Doe</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>29</v>
       </c>
@@ -2226,22 +2256,22 @@
         <v>John Doe</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="26"/>
+        <v>69</v>
+      </c>
+      <c r="G25" s="17"/>
       <c r="H25" s="16"/>
     </row>
-    <row r="26" spans="1:8" s="12" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>29</v>
       </c>
@@ -2250,24 +2280,22 @@
         <v>John Doe</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>80</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G26" s="26"/>
       <c r="H26" s="16"/>
     </row>
-    <row r="27" spans="1:8" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="12" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>29</v>
       </c>
@@ -2276,87 +2304,85 @@
         <v>John Doe</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="11">
         <f t="shared" si="3"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F27" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>John Doe</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" si="3"/>
+        <v>44531</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5" t="s">
+      <c r="G28" s="17"/>
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="4" t="s">
+      <c r="D29" s="5"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="9" t="str">
-        <f t="shared" ref="B29:B34" si="4">ExchangeTeam</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="str">
+        <f t="shared" ref="B30:B35" si="4">ExchangeTeam</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="11">
-        <f t="shared" ref="E29:E34" si="5">StartDate</f>
-        <v>43952</v>
-      </c>
-      <c r="F29" s="18" t="s">
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" ref="E30:E35" si="5">StartDate</f>
+        <v>44531</v>
+      </c>
+      <c r="F30" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v>John Doe</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="11">
-        <f t="shared" si="5"/>
-        <v>43952</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="H30" s="27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -2365,23 +2391,26 @@
         <v>John Doe</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="5"/>
-        <v>43952</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>88</v>
+        <v>44531</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>29</v>
       </c>
@@ -2390,23 +2419,23 @@
         <v>John Doe</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="11">
         <f t="shared" si="5"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>29</v>
       </c>
@@ -2415,23 +2444,23 @@
         <v>John Doe</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="11">
         <f t="shared" si="5"/>
-        <v>43952</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>91</v>
+        <v>44531</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>87</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>29</v>
       </c>
@@ -2440,65 +2469,62 @@
         <v>John Doe</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="11">
         <f t="shared" si="5"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F34" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>John Doe</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="11">
+        <f t="shared" si="5"/>
+        <v>44531</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G35" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5" t="s">
+    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="4" t="s">
+      <c r="D36" s="5"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="9" t="str">
-        <f>ExchangeTeam</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="11">
-        <f>StartDate</f>
-        <v>43952</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>29</v>
       </c>
@@ -2507,22 +2533,26 @@
         <v>John Doe</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
-    </row>
-    <row r="38" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>29</v>
       </c>
@@ -2531,24 +2561,22 @@
         <v>John Doe</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>103</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="G38" s="19"/>
       <c r="H38" s="20"/>
     </row>
-    <row r="39" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" s="12" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>29</v>
       </c>
@@ -2557,91 +2585,92 @@
         <v>John Doe</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F39" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="9" t="str">
+        <f>ExchangeTeam</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="11">
+        <f>StartDate</f>
+        <v>44531</v>
+      </c>
+      <c r="F40" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G40" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H39" s="20"/>
-    </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5" t="s">
+      <c r="H40" s="20"/>
+    </row>
+    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A41" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="9" t="str">
-        <f t="shared" ref="B41:B47" si="6">ExchangeTeam</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C41" s="10" t="s">
+      <c r="D41" s="5"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="9" t="str">
+        <f t="shared" ref="B42:B48" si="6">ExchangeTeam</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="11">
-        <f t="shared" ref="E41:E47" si="7">StartDate</f>
-        <v>43952</v>
-      </c>
-      <c r="F41" s="12" t="s">
+      <c r="D42" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="11">
+        <f t="shared" ref="E42:E48" si="7">StartDate</f>
+        <v>44531</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H42" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="G41" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>John Doe</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="11">
-        <f t="shared" si="7"/>
-        <v>43952</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="12" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>29</v>
       </c>
@@ -2650,26 +2679,23 @@
         <v>John Doe</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="7"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="12" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>29</v>
       </c>
@@ -2678,23 +2704,26 @@
         <v>John Doe</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="11">
         <f t="shared" si="7"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="G44" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>29</v>
       </c>
@@ -2703,26 +2732,23 @@
         <v>John Doe</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="11">
         <f t="shared" si="7"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" s="27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>29</v>
       </c>
@@ -2731,23 +2757,26 @@
         <v>John Doe</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="11">
         <f t="shared" si="7"/>
-        <v>43952</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>44531</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>29</v>
       </c>
@@ -2756,60 +2785,62 @@
         <v>John Doe</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="11">
         <f t="shared" si="7"/>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="F47" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>John Doe</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="11">
+        <f t="shared" si="7"/>
+        <v>44531</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="5" t="s">
+    </row>
+    <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="9" t="str">
-        <f>ExchangeTeam</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="11">
-        <f>StartDate</f>
-        <v>43952</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="5"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>29</v>
       </c>
@@ -2818,18 +2849,21 @@
         <v>John Doe</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="G50" s="19"/>
     </row>
-    <row r="51" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>29</v>
       </c>
@@ -2838,55 +2872,52 @@
         <v>John Doe</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="G51" s="19"/>
     </row>
-    <row r="52" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="5" t="s">
+    <row r="52" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="9" t="str">
+        <f>ExchangeTeam</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="11">
+        <f>StartDate</f>
+        <v>44531</v>
+      </c>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="9" t="str">
-        <f>ExchangeTeam</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="11">
-        <f>StartDate</f>
-        <v>43952</v>
-      </c>
-      <c r="F53" s="12" t="s">
+      <c r="D53" s="5"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G53" s="19"/>
-    </row>
-    <row r="54" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>29</v>
       </c>
@@ -2895,18 +2926,21 @@
         <v>John Doe</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="G54" s="19"/>
     </row>
-    <row r="55" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>29</v>
       </c>
@@ -2915,35 +2949,55 @@
         <v>John Doe</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="11">
         <f>StartDate</f>
-        <v>43952</v>
+        <v>44531</v>
       </c>
       <c r="G55" s="19"/>
+    </row>
+    <row r="56" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="9" t="str">
+        <f>ExchangeTeam</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="11">
+        <f>StartDate</f>
+        <v>44531</v>
+      </c>
+      <c r="G56" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15:D27 D3:D13" xr:uid="{9CF21033-E495-4A52-AEC8-2B2C7FBC45AB}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D28 D3:D14" xr:uid="{9CF21033-E495-4A52-AEC8-2B2C7FBC45AB}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H36" r:id="rId1" xr:uid="{8B84193D-7CE9-4E23-BA75-DF90E3B1F707}"/>
+    <hyperlink ref="H37" r:id="rId1" xr:uid="{8B84193D-7CE9-4E23-BA75-DF90E3B1F707}"/>
     <hyperlink ref="H5" r:id="rId2" xr:uid="{69FFDBB2-E364-48E4-9714-800F4AAFA8E5}"/>
     <hyperlink ref="H6" r:id="rId3" xr:uid="{FF8BE9E3-4ECA-4510-9658-37761269B8A3}"/>
     <hyperlink ref="H7" r:id="rId4" xr:uid="{BA640A13-D675-4150-B0B2-91378161D86A}"/>
     <hyperlink ref="H8" r:id="rId5" xr:uid="{CF6878A0-9680-49A9-B5CE-89F99FC628D7}"/>
-    <hyperlink ref="H30" r:id="rId6" xr:uid="{0B773944-DEAA-4C59-8024-E63FD5E4B49C}"/>
-    <hyperlink ref="H41" r:id="rId7" xr:uid="{0E4F173C-802B-460A-8373-10C3BCFC2F2B}"/>
-    <hyperlink ref="H45" r:id="rId8" xr:uid="{932D1C14-03F8-453B-971A-ADC931177C27}"/>
+    <hyperlink ref="H31" r:id="rId6" xr:uid="{0B773944-DEAA-4C59-8024-E63FD5E4B49C}"/>
+    <hyperlink ref="H42" r:id="rId7" xr:uid="{0E4F173C-802B-460A-8373-10C3BCFC2F2B}"/>
+    <hyperlink ref="H46" r:id="rId8" xr:uid="{932D1C14-03F8-453B-971A-ADC931177C27}"/>
     <hyperlink ref="H3" r:id="rId9" xr:uid="{A8767F7C-DC55-4811-A0C0-21CA973087DC}"/>
-    <hyperlink ref="H43" r:id="rId10" xr:uid="{D5787AF7-019E-44DB-BA66-089B427A77BA}"/>
+    <hyperlink ref="H44" r:id="rId10" xr:uid="{D5787AF7-019E-44DB-BA66-089B427A77BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
@@ -2959,27 +3013,27 @@
       <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Update Exchange Server 2019 Setup.xlsx
</commit_message>
<xml_diff>
--- a/Exchange Server 2019 Setup.xlsx
+++ b/Exchange Server 2019 Setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\SetupExchangeServer2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5866D3-64ED-4CB4-BE87-08F881A0D1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618F34E8-28AD-434C-A177-8F5529A204A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="22720" windowHeight="14480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="ResponsibleOnPremises">[1]Übersicht!$B$7</definedName>
     <definedName name="SourceName">[1]Übersicht!$B$3</definedName>
     <definedName name="StartDate">Übersicht!$B$10</definedName>
-    <definedName name="Status">Lookup!$A$3:$A$5</definedName>
+    <definedName name="Status">Lookup!$A$3:$A$6</definedName>
     <definedName name="TargetName">[1]Übersicht!$B$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="145">
   <si>
     <t>Plattform</t>
   </si>
@@ -455,32 +455,6 @@
     <t>2.4</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Einspieling der .reg Dateien aus </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> zur Anpassung der Windows Registry für Best Practices</t>
-    </r>
-  </si>
-  <si>
     <t>Neustart des Servers</t>
   </si>
   <si>
@@ -864,6 +838,35 @@
   </si>
   <si>
     <t>Setup.exe /PrepareAllDomains /IAcceptExchangeServerLicenseTerms_DiagnosticDataOFF</t>
+  </si>
+  <si>
+    <t>Nicht notwendig</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Einspielung der .reg Dateien aus </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zur Anpassung der Windows Registry für Best Practices</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1611,17 +1614,17 @@
     </row>
     <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="str">
-        <f>Lookup!A5</f>
-        <v>Abgeschlossen</v>
+        <f>Lookup!A6</f>
+        <v>Nicht notwendig</v>
       </c>
       <c r="B16" s="25">
-        <f>COUNTIF('Installation Exchange 2019'!D:D,Lookup!A5)</f>
+        <f>COUNTIF('Installation Exchange 2019'!D:D,Lookup!A6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>7</v>
@@ -1650,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CACAE57-EC22-477C-B012-303C9CEF819F}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,7 +1688,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1725,11 +1728,11 @@
         <v>44531</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L3" s="14"/>
     </row>
@@ -1752,7 +1755,7 @@
         <v>44531</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="13"/>
       <c r="L4" s="14"/>
@@ -1884,11 +1887,11 @@
         <v>44531</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L9" s="14"/>
     </row>
@@ -1928,7 +1931,7 @@
         <v>John Doe</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>8</v>
@@ -1942,7 +1945,7 @@
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L11" s="14"/>
     </row>
@@ -1955,7 +1958,7 @@
         <v>John Doe</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>8</v>
@@ -1978,7 +1981,7 @@
         <v>John Doe</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>8</v>
@@ -1988,7 +1991,7 @@
         <v>44531</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G13" s="13"/>
     </row>
@@ -2001,7 +2004,7 @@
         <v>John Doe</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>8</v>
@@ -2011,7 +2014,7 @@
         <v>44531</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" s="13"/>
     </row>
@@ -2024,7 +2027,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="15"/>
       <c r="F15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -2062,7 +2065,7 @@
         <v>John Doe</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>8</v>
@@ -2088,7 +2091,7 @@
         <v>John Doe</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>8</v>
@@ -2148,7 +2151,7 @@
         <v>44531</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="16"/>
@@ -2162,7 +2165,7 @@
         <v>John Doe</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>8</v>
@@ -2172,10 +2175,10 @@
         <v>44531</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H21" s="16"/>
     </row>
@@ -2188,7 +2191,7 @@
         <v>John Doe</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>8</v>
@@ -2198,7 +2201,7 @@
         <v>44531</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="16"/>
@@ -2212,7 +2215,7 @@
         <v>John Doe</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>8</v>
@@ -2222,7 +2225,7 @@
         <v>44531</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="16"/>
@@ -2236,7 +2239,7 @@
         <v>John Doe</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>8</v>
@@ -2246,10 +2249,10 @@
         <v>44531</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" s="16"/>
     </row>
@@ -2262,7 +2265,7 @@
         <v>John Doe</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>8</v>
@@ -2272,7 +2275,7 @@
         <v>44531</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="16"/>
@@ -2286,7 +2289,7 @@
         <v>John Doe</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>8</v>
@@ -2296,7 +2299,7 @@
         <v>44531</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="26"/>
       <c r="H26" s="16"/>
@@ -2310,7 +2313,7 @@
         <v>John Doe</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>8</v>
@@ -2320,10 +2323,10 @@
         <v>44531</v>
       </c>
       <c r="F27" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="H27" s="16"/>
     </row>
@@ -2336,7 +2339,7 @@
         <v>John Doe</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>8</v>
@@ -2346,7 +2349,7 @@
         <v>44531</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="16"/>
@@ -2360,7 +2363,7 @@
         <v>John Doe</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>8</v>
@@ -2370,7 +2373,7 @@
         <v>44531</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="16"/>
@@ -2384,7 +2387,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="15"/>
       <c r="F30" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -2408,7 +2411,7 @@
         <v>44531</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G31" s="13"/>
     </row>
@@ -2431,13 +2434,13 @@
         <v>44531</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2449,7 +2452,7 @@
         <v>John Doe</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>8</v>
@@ -2459,10 +2462,10 @@
         <v>44531</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2474,7 +2477,7 @@
         <v>John Doe</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>8</v>
@@ -2484,10 +2487,10 @@
         <v>44531</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2499,7 +2502,7 @@
         <v>John Doe</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>8</v>
@@ -2509,10 +2512,10 @@
         <v>44531</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2524,7 +2527,7 @@
         <v>John Doe</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>8</v>
@@ -2534,10 +2537,10 @@
         <v>44531</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2573,10 +2576,10 @@
         <v>44531</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>19</v>
@@ -2591,7 +2594,7 @@
         <v>John Doe</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>8</v>
@@ -2601,7 +2604,7 @@
         <v>44531</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
@@ -2615,7 +2618,7 @@
         <v>John Doe</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>8</v>
@@ -2625,10 +2628,10 @@
         <v>44531</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H40" s="20"/>
     </row>
@@ -2641,7 +2644,7 @@
         <v>John Doe</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>8</v>
@@ -2651,10 +2654,10 @@
         <v>44531</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H41" s="20"/>
     </row>
@@ -2667,7 +2670,7 @@
       <c r="D42" s="5"/>
       <c r="E42" s="15"/>
       <c r="F42" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -2691,13 +2694,13 @@
         <v>44531</v>
       </c>
       <c r="F43" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" s="16" t="s">
         <v>101</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2719,10 +2722,10 @@
         <v>44531</v>
       </c>
       <c r="F44" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" s="19" t="s">
         <v>104</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="12" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
@@ -2744,13 +2747,13 @@
         <v>44531</v>
       </c>
       <c r="F45" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G45" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="H45" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2772,10 +2775,10 @@
         <v>44531</v>
       </c>
       <c r="F46" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2787,7 +2790,7 @@
         <v>John Doe</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>8</v>
@@ -2797,13 +2800,13 @@
         <v>44531</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G47" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H47" s="27" t="s">
         <v>112</v>
-      </c>
-      <c r="H47" s="27" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2815,7 +2818,7 @@
         <v>John Doe</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>8</v>
@@ -2825,10 +2828,10 @@
         <v>44531</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -2840,7 +2843,7 @@
         <v>John Doe</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>8</v>
@@ -2850,10 +2853,10 @@
         <v>44531</v>
       </c>
       <c r="F49" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G49" s="28" t="s">
         <v>115</v>
-      </c>
-      <c r="G49" s="28" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2865,7 +2868,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="15"/>
       <c r="F50" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -2889,7 +2892,7 @@
         <v>44531</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G51" s="19"/>
     </row>
@@ -2942,7 +2945,7 @@
       <c r="D54" s="5"/>
       <c r="E54" s="15"/>
       <c r="F54" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -2966,7 +2969,7 @@
         <v>44531</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G55" s="19"/>
     </row>
@@ -3012,8 +3015,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D14 D16:D29" xr:uid="{9CF21033-E495-4A52-AEC8-2B2C7FBC45AB}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D14 D16:D29 D31:D36 D38:D41 D43:D49 D51:D53 D55:D57" xr:uid="{9CF21033-E495-4A52-AEC8-2B2C7FBC45AB}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -3037,15 +3040,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5D6F62-C56B-4C32-97FB-610135D5668E}">
-  <dimension ref="A2:A5"/>
+  <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -3068,6 +3071,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>